<commit_message>
New Code For Pages
</commit_message>
<xml_diff>
--- a/ApplicationTestData/ScPages.xlsx
+++ b/ApplicationTestData/ScPages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Urls" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Title</t>
   </si>
@@ -60,9 +60,6 @@
     <t>campaign-page</t>
   </si>
   <si>
-    <t xml:space="preserve">Test Content Page Test </t>
-  </si>
-  <si>
     <t>Véhicules neufs</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>Evènements VN</t>
   </si>
   <si>
-    <t xml:space="preserve">Test CampaignPage Test </t>
-  </si>
-  <si>
     <t>SpecialPage</t>
   </si>
   <si>
@@ -87,14 +81,38 @@
     <t>Evènements APV</t>
   </si>
   <si>
-    <t>Special Page Content</t>
+    <t>AboutUsPage</t>
+  </si>
+  <si>
+    <t>aboutus-page</t>
+  </si>
+  <si>
+    <t>Pièces de rechange</t>
+  </si>
+  <si>
+    <t>About us Page test data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special Page Content data </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test CampaignPage Test  data </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Content Page Test data  </t>
+  </si>
+  <si>
+    <t>https://qadealeradminv2fr.izmocars.com/updatePageUrlsByLevelAuth.htm</t>
+  </si>
+  <si>
+    <t>http://citroen-annecy.stg-eudemosite.com/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,8 +120,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,6 +147,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -132,18 +163,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -476,15 +515,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="1" max="1" width="69.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" s="2" customFormat="1">
@@ -493,21 +532,34 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -515,11 +567,12 @@
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -548,11 +601,11 @@
         <v>11</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -567,7 +620,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>3</v>
@@ -581,18 +634,18 @@
         <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="D7" s="5"/>
     </row>
@@ -607,7 +660,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>3</v>
@@ -615,19 +668,52 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="5" t="s">
+    </row>
+    <row r="11" spans="1:5" s="1" customFormat="1">
+      <c r="A11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="E9" t="s">
+      <c r="C12" t="s">
         <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>